<commit_message>
Reports in out.py - Extended the number of reports Functions created for report and plot creation Moved these functions to out.py Extended the number of reports and plots to depict correlations
</commit_message>
<xml_diff>
--- a/out/factors.xlsx
+++ b/out/factors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,11 +474,6 @@
           <t>feature_importance</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>predicted_dissatisfaction_delta</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -511,9 +506,6 @@
       <c r="H2" t="n">
         <v>0.9015337936114683</v>
       </c>
-      <c r="I2" t="n">
-        <v>0.04905457279069363</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -546,9 +538,6 @@
       <c r="H3" t="n">
         <v>0.04199055645104691</v>
       </c>
-      <c r="I3" t="n">
-        <v>0.02656152611675559</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -581,9 +570,6 @@
       <c r="H4" t="n">
         <v>0.02509623056070723</v>
       </c>
-      <c r="I4" t="n">
-        <v>0.01880236057734017</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -616,18 +602,15 @@
       <c r="H5" t="n">
         <v>0.007007616490164711</v>
       </c>
-      <c r="I5" t="n">
-        <v>0.0111501935098194</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>caller_is_employee</t>
+          <t>reassignment_count</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -640,29 +623,26 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F6" t="n">
-        <v>85.03539735886675</v>
+        <v>384.3171526993451</v>
       </c>
       <c r="G6" t="n">
-        <v>2.930712052604616e-20</v>
+        <v>1.358657888241235e-72</v>
       </c>
       <c r="H6" t="n">
-        <v>0.005773965052043</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.01078907443846973</v>
+        <v>0.006951365941291337</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>reassignment_count</t>
+          <t>caller_is_employee</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -675,19 +655,16 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
-        <v>384.3171526993451</v>
+        <v>85.03539735886675</v>
       </c>
       <c r="G7" t="n">
-        <v>1.358657888241235e-72</v>
+        <v>2.930712052604616e-20</v>
       </c>
       <c r="H7" t="n">
-        <v>0.006951365941291337</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.00188231226842886</v>
+        <v>0.005773965052043</v>
       </c>
     </row>
     <row r="8">
@@ -721,7 +698,6 @@
       <c r="H8" t="n">
         <v>0.005488917236315931</v>
       </c>
-      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -754,7 +730,6 @@
       <c r="H9" t="n">
         <v>0.002531471778483367</v>
       </c>
-      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -787,7 +762,6 @@
       <c r="H10" t="n">
         <v>0.002124437843850688</v>
       </c>
-      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -820,7 +794,6 @@
       <c r="H11" t="n">
         <v>0.0008014904885535787</v>
       </c>
-      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -853,7 +826,6 @@
       <c r="H12" t="n">
         <v>0.0007001545460747457</v>
       </c>
-      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -886,7 +858,6 @@
       <c r="H13" t="n">
         <v>0</v>
       </c>
-      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -919,7 +890,6 @@
       <c r="H14" t="n">
         <v>0</v>
       </c>
-      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -952,7 +922,6 @@
       <c r="H15" t="n">
         <v>0</v>
       </c>
-      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -985,7 +954,6 @@
       <c r="H16" t="n">
         <v>0</v>
       </c>
-      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1014,7 +982,6 @@
         <v>6.281977847913644e-23</v>
       </c>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1043,7 +1010,6 @@
         <v>9.202799494861961e-76</v>
       </c>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1072,7 +1038,6 @@
         <v>1.055341826075107e-94</v>
       </c>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1101,7 +1066,6 @@
         <v>1.400057343459844e-66</v>
       </c>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1130,7 +1094,6 @@
         <v>5.492938861828806e-18</v>
       </c>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1159,7 +1122,6 @@
         <v>3.533923241743454e-15</v>
       </c>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1188,7 +1150,6 @@
         <v>1.009852580679422e-07</v>
       </c>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1217,7 +1178,6 @@
         <v>1.464738759557574e-05</v>
       </c>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1246,7 +1206,6 @@
         <v>0.6220148571644246</v>
       </c>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1271,7 +1230,6 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>